<commit_message>
deleted and moved some files
</commit_message>
<xml_diff>
--- a/src/run_data.xlsx
+++ b/src/run_data.xlsx
@@ -2667,7 +2667,7 @@
         <v>19546</v>
       </c>
       <c r="M47" t="n">
-        <v>0.0279</v>
+        <v>0.0278</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -2676,7 +2676,7 @@
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>10:53:53</t>
+          <t>10:59:04</t>
         </is>
       </c>
     </row>

</xml_diff>